<commit_message>
Added graphs to results
</commit_message>
<xml_diff>
--- a/test/Results.xlsx
+++ b/test/Results.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5927646E-1342-4FB6-B6C9-8D7D45E5671E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C162DA26-097B-4A3F-896A-AE70BCFA4659}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2865" yWindow="2850" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2865" yWindow="2850" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DP" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
   <si>
     <t xml:space="preserve"> Input n =</t>
   </si>
@@ -42,6 +42,12 @@
   </si>
   <si>
     <t>seconds</t>
+  </si>
+  <si>
+    <t>Case n =</t>
+  </si>
+  <si>
+    <t>Average time in seconds (DP)</t>
   </si>
 </sst>
 </file>
@@ -103,6 +109,3021 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="nl-NL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>DP, n = 2 until 15</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>DP!$A$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average time in seconds (DP)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>DP!$B$23:$O$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>DP!$B$24:$O$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0.10711662</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.10175886000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.10306912999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.10178466</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.10230370999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.10212934999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.10196727000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.10202625000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.10247448000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.10318823000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.1039153</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.10435120000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.10540279000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.1101707</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-645D-4568-9E99-B4BA3F6001AB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="447776864"/>
+        <c:axId val="447769320"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="447776864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nl-NL"/>
+                  <a:t>Case</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="nl-NL" baseline="0"/>
+                  <a:t> n = </a:t>
+                </a:r>
+                <a:endParaRPr lang="nl-NL"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="nl-NL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="447769320"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="447769320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nl-NL"/>
+                  <a:t>Average</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="nl-NL" baseline="0"/>
+                  <a:t> ti</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="nl-NL"/>
+                  <a:t>me in seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="nl-NL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="447776864"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="nl-NL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="nl-NL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>DP,</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> n = 15 until 20</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>DP!$A$27</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average time in seconds (DP)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>DP!$B$26:$G$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>DP!$B$27:$G$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.1101707</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.12305466000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.13682078000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.18200585000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.25607721999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.47030666999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E077-473F-B3FB-96E58948EB10}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="451980832"/>
+        <c:axId val="451978208"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="451980832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nl-NL"/>
+                  <a:t>Case n = </a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="nl-NL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="451978208"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="451978208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nl-NL"/>
+                  <a:t>Average time in seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="nl-NL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="451980832"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="nl-NL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="nl-NL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="nl-NL"/>
+              <a:t>DP, n = 20 until 27</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>DP!$A$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average time in seconds (DP)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>DP!$B$29:$I$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>27</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>DP!$B$30:$I$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.47030666999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.84625224999999982</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.23276578</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5754002900000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.8702807000000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.614377210000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>28.376700540000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>71.211102479999994</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C4EC-4758-B6F7-9210FC079181}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="455988600"/>
+        <c:axId val="455990240"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="455988600"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="455990240"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="455990240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="455988600"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="nl-NL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Grafiek 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50EEA7B4-DD37-47C4-AB14-72AE6D90AB75}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>290512</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>595312</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Grafiek 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{302CF627-ED62-42CC-A11F-DDBE362D70D8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>490537</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>185737</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Grafiek 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB941104-1B1A-4422-8BE8-B40BAD4E9F18}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -368,10 +3389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD14"/>
+  <dimension ref="A1:AD30"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+    <sheetView tabSelected="1" topLeftCell="C37" workbookViewId="0">
+      <selection activeCell="K56" sqref="K56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1426,8 +4447,373 @@
         <v>#DIV/0!</v>
       </c>
     </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="1">
+        <v>2</v>
+      </c>
+      <c r="C23" s="1">
+        <f>B23+1</f>
+        <v>3</v>
+      </c>
+      <c r="D23" s="1">
+        <f t="shared" ref="D23" si="2">C23+1</f>
+        <v>4</v>
+      </c>
+      <c r="E23" s="1">
+        <f t="shared" ref="E23" si="3">D23+1</f>
+        <v>5</v>
+      </c>
+      <c r="F23" s="1">
+        <f t="shared" ref="F23" si="4">E23+1</f>
+        <v>6</v>
+      </c>
+      <c r="G23" s="1">
+        <f t="shared" ref="G23" si="5">F23+1</f>
+        <v>7</v>
+      </c>
+      <c r="H23" s="1">
+        <f t="shared" ref="H23" si="6">G23+1</f>
+        <v>8</v>
+      </c>
+      <c r="I23" s="1">
+        <f t="shared" ref="I23" si="7">H23+1</f>
+        <v>9</v>
+      </c>
+      <c r="J23" s="1">
+        <f t="shared" ref="J23" si="8">I23+1</f>
+        <v>10</v>
+      </c>
+      <c r="K23" s="1">
+        <f t="shared" ref="K23" si="9">J23+1</f>
+        <v>11</v>
+      </c>
+      <c r="L23" s="1">
+        <f t="shared" ref="L23" si="10">K23+1</f>
+        <v>12</v>
+      </c>
+      <c r="M23" s="1">
+        <f t="shared" ref="M23" si="11">L23+1</f>
+        <v>13</v>
+      </c>
+      <c r="N23" s="1">
+        <f t="shared" ref="N23" si="12">M23+1</f>
+        <v>14</v>
+      </c>
+      <c r="O23" s="1">
+        <f t="shared" ref="O23" si="13">N23+1</f>
+        <v>15</v>
+      </c>
+      <c r="P23" s="1">
+        <f t="shared" ref="P23" si="14">O23+1</f>
+        <v>16</v>
+      </c>
+      <c r="Q23" s="1">
+        <f t="shared" ref="Q23" si="15">P23+1</f>
+        <v>17</v>
+      </c>
+      <c r="R23" s="1">
+        <f t="shared" ref="R23" si="16">Q23+1</f>
+        <v>18</v>
+      </c>
+      <c r="S23" s="1">
+        <f t="shared" ref="S23" si="17">R23+1</f>
+        <v>19</v>
+      </c>
+      <c r="T23" s="1">
+        <f t="shared" ref="T23" si="18">S23+1</f>
+        <v>20</v>
+      </c>
+      <c r="U23" s="1">
+        <f t="shared" ref="U23" si="19">T23+1</f>
+        <v>21</v>
+      </c>
+      <c r="V23" s="1">
+        <f t="shared" ref="V23" si="20">U23+1</f>
+        <v>22</v>
+      </c>
+      <c r="W23" s="1">
+        <f t="shared" ref="W23" si="21">V23+1</f>
+        <v>23</v>
+      </c>
+      <c r="X23" s="1">
+        <f t="shared" ref="X23" si="22">W23+1</f>
+        <v>24</v>
+      </c>
+      <c r="Y23" s="1">
+        <f>X23+1</f>
+        <v>25</v>
+      </c>
+      <c r="Z23" s="1">
+        <f t="shared" ref="Z23" si="23">Y23+1</f>
+        <v>26</v>
+      </c>
+      <c r="AA23" s="1">
+        <f t="shared" ref="AA23" si="24">Z23+1</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24">
+        <f>SUM(B13:B22)/COUNT(B13:B22)</f>
+        <v>0.10711662</v>
+      </c>
+      <c r="C24">
+        <f t="shared" ref="C24:AA24" si="25">SUM(C13:C22)/COUNT(C13:C22)</f>
+        <v>0.10175886000000001</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="25"/>
+        <v>0.10306912999999999</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="25"/>
+        <v>0.10178466</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="25"/>
+        <v>0.10230370999999998</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="25"/>
+        <v>0.10212934999999998</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="25"/>
+        <v>0.10196727000000001</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="25"/>
+        <v>0.10202625000000001</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="25"/>
+        <v>0.10247448000000001</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="25"/>
+        <v>0.10318823000000002</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="25"/>
+        <v>0.1039153</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="25"/>
+        <v>0.10435120000000001</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="25"/>
+        <v>0.10540279000000001</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="25"/>
+        <v>0.1101707</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="25"/>
+        <v>0.12305466000000001</v>
+      </c>
+      <c r="Q24">
+        <f t="shared" si="25"/>
+        <v>0.13682078000000003</v>
+      </c>
+      <c r="R24">
+        <f t="shared" si="25"/>
+        <v>0.18200585000000002</v>
+      </c>
+      <c r="S24">
+        <f t="shared" si="25"/>
+        <v>0.25607721999999999</v>
+      </c>
+      <c r="T24">
+        <f t="shared" si="25"/>
+        <v>0.47030666999999998</v>
+      </c>
+      <c r="U24">
+        <f t="shared" si="25"/>
+        <v>0.84625224999999982</v>
+      </c>
+      <c r="V24">
+        <f t="shared" si="25"/>
+        <v>1.23276578</v>
+      </c>
+      <c r="W24">
+        <f t="shared" si="25"/>
+        <v>2.5754002900000001</v>
+      </c>
+      <c r="X24">
+        <f t="shared" si="25"/>
+        <v>4.8702807000000004</v>
+      </c>
+      <c r="Y24">
+        <f t="shared" si="25"/>
+        <v>12.614377210000001</v>
+      </c>
+      <c r="Z24">
+        <f t="shared" si="25"/>
+        <v>28.376700540000002</v>
+      </c>
+      <c r="AA24">
+        <f t="shared" si="25"/>
+        <v>71.211102479999994</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="1">
+        <v>15</v>
+      </c>
+      <c r="C26" s="1">
+        <v>16</v>
+      </c>
+      <c r="D26" s="1">
+        <v>17</v>
+      </c>
+      <c r="E26" s="1">
+        <v>18</v>
+      </c>
+      <c r="F26" s="1">
+        <v>19</v>
+      </c>
+      <c r="G26" s="1">
+        <v>20</v>
+      </c>
+      <c r="H26" s="1">
+        <v>21</v>
+      </c>
+      <c r="I26" s="1">
+        <v>22</v>
+      </c>
+      <c r="J26" s="1">
+        <v>23</v>
+      </c>
+      <c r="K26" s="1">
+        <v>24</v>
+      </c>
+      <c r="L26" s="1">
+        <v>25</v>
+      </c>
+      <c r="M26" s="1">
+        <v>26</v>
+      </c>
+      <c r="N26" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27">
+        <v>0.1101707</v>
+      </c>
+      <c r="C27">
+        <v>0.12305466000000001</v>
+      </c>
+      <c r="D27">
+        <v>0.13682078000000003</v>
+      </c>
+      <c r="E27">
+        <v>0.18200585000000002</v>
+      </c>
+      <c r="F27">
+        <v>0.25607721999999999</v>
+      </c>
+      <c r="G27">
+        <v>0.47030666999999998</v>
+      </c>
+      <c r="H27">
+        <v>0.84625224999999982</v>
+      </c>
+      <c r="I27">
+        <v>1.23276578</v>
+      </c>
+      <c r="J27">
+        <v>2.5754002900000001</v>
+      </c>
+      <c r="K27">
+        <v>4.8702807000000004</v>
+      </c>
+      <c r="L27">
+        <v>12.614377210000001</v>
+      </c>
+      <c r="M27">
+        <v>28.376700540000002</v>
+      </c>
+      <c r="N27">
+        <v>71.211102479999994</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="1">
+        <v>20</v>
+      </c>
+      <c r="C29" s="1">
+        <v>21</v>
+      </c>
+      <c r="D29" s="1">
+        <v>22</v>
+      </c>
+      <c r="E29" s="1">
+        <v>23</v>
+      </c>
+      <c r="F29" s="1">
+        <v>24</v>
+      </c>
+      <c r="G29" s="1">
+        <v>25</v>
+      </c>
+      <c r="H29" s="1">
+        <v>26</v>
+      </c>
+      <c r="I29" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30">
+        <v>0.47030666999999998</v>
+      </c>
+      <c r="C30">
+        <v>0.84625224999999982</v>
+      </c>
+      <c r="D30">
+        <v>1.23276578</v>
+      </c>
+      <c r="E30">
+        <v>2.5754002900000001</v>
+      </c>
+      <c r="F30">
+        <v>4.8702807000000004</v>
+      </c>
+      <c r="G30">
+        <v>12.614377210000001</v>
+      </c>
+      <c r="H30">
+        <v>28.376700540000002</v>
+      </c>
+      <c r="I30">
+        <v>71.211102479999994</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1435,8 +4821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3726C64E-E8AE-4B79-ABC5-C32566F621D9}">
   <dimension ref="A1:AD14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AD3" sqref="AD3:AD12"/>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="T18" sqref="T18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Created table of results of time in ms
</commit_message>
<xml_diff>
--- a/test/Results.xlsx
+++ b/test/Results.xlsx
@@ -3,13 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C162DA26-097B-4A3F-896A-AE70BCFA4659}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D01EBB6-586B-4733-A67B-E34CAACAB1B9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2865" yWindow="2850" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2865" yWindow="2850" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="DP" sheetId="1" r:id="rId1"/>
-    <sheet name="BF" sheetId="2" r:id="rId2"/>
+    <sheet name="DP Raw results + graphs" sheetId="1" r:id="rId1"/>
+    <sheet name="DP Table of results" sheetId="4" r:id="rId2"/>
+    <sheet name="BF" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
   <si>
     <t xml:space="preserve"> Input n =</t>
   </si>
@@ -48,6 +49,15 @@
   </si>
   <si>
     <t>Average time in seconds (DP)</t>
+  </si>
+  <si>
+    <t>Average time in milliseconds (DP)</t>
+  </si>
+  <si>
+    <t>Out of memory error (sometimes)</t>
+  </si>
+  <si>
+    <t>Not tested</t>
   </si>
 </sst>
 </file>
@@ -192,7 +202,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>DP!$A$24</c:f>
+              <c:f>'DP Raw results + graphs'!$A$24</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -213,7 +223,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>DP!$B$23:$O$23</c:f>
+              <c:f>'DP Raw results + graphs'!$B$23:$O$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -264,7 +274,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>DP!$B$24:$O$24</c:f>
+              <c:f>'DP Raw results + graphs'!$B$24:$O$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -693,7 +703,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>DP!$A$27</c:f>
+              <c:f>'DP Raw results + graphs'!$A$27</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -714,7 +724,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>DP!$B$26:$G$26</c:f>
+              <c:f>'DP Raw results + graphs'!$B$26:$G$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -741,7 +751,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>DP!$B$27:$G$27</c:f>
+              <c:f>'DP Raw results + graphs'!$B$27:$G$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1128,7 +1138,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>DP!$A$30</c:f>
+              <c:f>'DP Raw results + graphs'!$A$30</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1149,7 +1159,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>DP!$B$29:$I$29</c:f>
+              <c:f>'DP Raw results + graphs'!$B$29:$I$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1182,7 +1192,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>DP!$B$30:$I$30</c:f>
+              <c:f>'DP Raw results + graphs'!$B$30:$I$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3391,8 +3401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C37" workbookViewId="0">
-      <selection activeCell="K56" sqref="K56"/>
+    <sheetView topLeftCell="J19" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:AA24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4818,6 +4828,267 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86B2FD24-48B6-4D33-AC11-A86A9E1FB876}">
+  <dimension ref="A1:C30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="32.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>22</v>
+      </c>
+      <c r="B22">
+        <v>1233</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>23</v>
+      </c>
+      <c r="B23">
+        <v>2575</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>24</v>
+      </c>
+      <c r="B24">
+        <v>4870</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>25</v>
+      </c>
+      <c r="B25">
+        <v>12614</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>26</v>
+      </c>
+      <c r="B26">
+        <v>28377</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>27</v>
+      </c>
+      <c r="B27">
+        <v>71211</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>28</v>
+      </c>
+      <c r="B28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>29</v>
+      </c>
+      <c r="B29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>30</v>
+      </c>
+      <c r="B30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3726C64E-E8AE-4B79-ABC5-C32566F621D9}">
   <dimension ref="A1:AD14"/>
   <sheetViews>

</xml_diff>

<commit_message>
Retested BF after bugfix for n = 25 until 30, added table.
</commit_message>
<xml_diff>
--- a/test/Results.xlsx
+++ b/test/Results.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D01EBB6-586B-4733-A67B-E34CAACAB1B9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{250F63CB-4952-43A4-92AF-57BA40C638EF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2865" yWindow="2850" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2865" yWindow="2850" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="DP Raw results + graphs" sheetId="1" r:id="rId1"/>
-    <sheet name="DP Table of results" sheetId="4" r:id="rId2"/>
-    <sheet name="BF" sheetId="2" r:id="rId3"/>
+    <sheet name="DP - Random - Raw results+graph" sheetId="1" r:id="rId1"/>
+    <sheet name="DP - Random - Table of results" sheetId="4" r:id="rId2"/>
+    <sheet name="BF - Random - Raw results" sheetId="2" r:id="rId3"/>
+    <sheet name="BF - Random - Table of results" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
   <si>
     <t xml:space="preserve"> Input n =</t>
   </si>
@@ -58,6 +59,9 @@
   </si>
   <si>
     <t>Not tested</t>
+  </si>
+  <si>
+    <t>Average time in milliseconds (BF)</t>
   </si>
 </sst>
 </file>
@@ -202,7 +206,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'DP Raw results + graphs'!$A$24</c:f>
+              <c:f>'DP - Random - Raw results+graph'!$A$24</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -223,7 +227,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'DP Raw results + graphs'!$B$23:$O$23</c:f>
+              <c:f>'DP - Random - Raw results+graph'!$B$23:$O$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -274,7 +278,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'DP Raw results + graphs'!$B$24:$O$24</c:f>
+              <c:f>'DP - Random - Raw results+graph'!$B$24:$O$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -703,7 +707,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'DP Raw results + graphs'!$A$27</c:f>
+              <c:f>'DP - Random - Raw results+graph'!$A$27</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -724,7 +728,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'DP Raw results + graphs'!$B$26:$G$26</c:f>
+              <c:f>'DP - Random - Raw results+graph'!$B$26:$G$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -751,7 +755,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'DP Raw results + graphs'!$B$27:$G$27</c:f>
+              <c:f>'DP - Random - Raw results+graph'!$B$27:$G$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1138,7 +1142,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'DP Raw results + graphs'!$A$30</c:f>
+              <c:f>'DP - Random - Raw results+graph'!$A$30</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1159,7 +1163,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'DP Raw results + graphs'!$B$29:$I$29</c:f>
+              <c:f>'DP - Random - Raw results+graph'!$B$29:$I$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1192,7 +1196,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'DP Raw results + graphs'!$B$30:$I$30</c:f>
+              <c:f>'DP - Random - Raw results+graph'!$B$30:$I$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3401,8 +3405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD30"/>
   <sheetViews>
-    <sheetView topLeftCell="J19" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:AA24"/>
+    <sheetView topLeftCell="D7" workbookViewId="0">
+      <selection activeCell="O35" sqref="O35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4831,8 +4835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86B2FD24-48B6-4D33-AC11-A86A9E1FB876}">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5090,1143 +5094,418 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3726C64E-E8AE-4B79-ABC5-C32566F621D9}">
-  <dimension ref="A1:AD14"/>
+  <dimension ref="A1:X18"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="T18" sqref="T18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1">
         <f>B1+1</f>
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="D1" s="1">
-        <f t="shared" ref="D1:AD1" si="0">C1+1</f>
-        <v>4</v>
+        <f>C1+1</f>
+        <v>27</v>
       </c>
       <c r="E1" s="1">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f>D1+1</f>
+        <v>28</v>
       </c>
       <c r="F1" s="1">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f>E1+1</f>
+        <v>29</v>
       </c>
       <c r="G1" s="1">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="H1" s="1">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="I1" s="1">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="J1" s="1">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="K1" s="1">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="L1" s="1">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="M1" s="1">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="N1" s="1">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="O1" s="1">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="P1" s="1">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="Q1" s="1">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="R1" s="1">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="S1" s="1">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="T1" s="1">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="U1" s="1">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="V1" s="1">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="W1" s="1">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="X1" s="1">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="Y1" s="1">
-        <f>X1+1</f>
-        <v>25</v>
-      </c>
-      <c r="Z1" s="1">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="AA1" s="1">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="AB1" s="1">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="AC1" s="1">
-        <f>AB1+1</f>
-        <v>29</v>
-      </c>
-      <c r="AD1" s="1">
-        <f t="shared" si="0"/>
+        <f>F1+1</f>
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B3">
-        <v>9.8360400000000001E-2</v>
+        <v>0.1052882</v>
       </c>
       <c r="C3">
-        <v>9.7610699999999995E-2</v>
+        <v>0.1026234</v>
       </c>
       <c r="D3">
-        <v>9.6685300000000002E-2</v>
+        <v>0.10568279999999999</v>
       </c>
       <c r="E3">
-        <v>9.7248699999999993E-2</v>
+        <v>0.10151640000000001</v>
       </c>
       <c r="F3">
-        <v>9.44073E-2</v>
+        <v>0.10290059999999999</v>
       </c>
       <c r="G3">
-        <v>9.9578100000000003E-2</v>
-      </c>
-      <c r="H3">
-        <v>9.5084600000000005E-2</v>
-      </c>
-      <c r="I3">
-        <v>9.5993499999999995E-2</v>
-      </c>
-      <c r="J3">
-        <v>0.10058640000000001</v>
-      </c>
-      <c r="K3">
-        <v>0.1012617</v>
-      </c>
-      <c r="L3">
-        <v>0.102968</v>
-      </c>
-      <c r="M3">
-        <v>9.89564E-2</v>
-      </c>
-      <c r="N3">
-        <v>9.9449300000000004E-2</v>
-      </c>
-      <c r="O3">
-        <v>9.8704299999999995E-2</v>
-      </c>
-      <c r="P3">
-        <v>9.8454E-2</v>
-      </c>
-      <c r="Q3">
-        <v>9.8054500000000003E-2</v>
-      </c>
-      <c r="R3">
-        <v>9.8302500000000001E-2</v>
-      </c>
-      <c r="S3">
-        <v>0.1037338</v>
-      </c>
-      <c r="T3">
-        <v>0.10311620000000001</v>
-      </c>
-      <c r="U3">
-        <v>0.1026687</v>
-      </c>
-      <c r="V3">
-        <v>9.9756899999999996E-2</v>
-      </c>
-      <c r="W3">
-        <v>0.1015508</v>
-      </c>
-      <c r="X3">
-        <v>9.88541E-2</v>
-      </c>
-      <c r="Y3">
-        <v>9.9790699999999996E-2</v>
-      </c>
-      <c r="Z3">
-        <v>9.8685099999999998E-2</v>
-      </c>
-      <c r="AA3">
-        <v>0.1002171</v>
-      </c>
-      <c r="AB3">
-        <v>0.1020433</v>
-      </c>
-      <c r="AC3">
-        <v>0.1017347</v>
-      </c>
-      <c r="AD3">
-        <v>0.1002063</v>
-      </c>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+        <v>0.10300570000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B4">
-        <v>9.393E-2</v>
+        <v>0.100568</v>
       </c>
       <c r="C4">
-        <v>9.8745700000000006E-2</v>
+        <v>0.1006715</v>
       </c>
       <c r="D4">
-        <v>9.8321699999999998E-2</v>
+        <v>0.10099130000000001</v>
       </c>
       <c r="E4">
-        <v>9.8497299999999996E-2</v>
+        <v>0.10411769999999999</v>
       </c>
       <c r="F4">
-        <v>9.5214300000000002E-2</v>
+        <v>0.10028040000000001</v>
       </c>
       <c r="G4">
-        <v>0.10293190000000001</v>
-      </c>
-      <c r="H4">
-        <v>9.7870100000000002E-2</v>
-      </c>
-      <c r="I4">
-        <v>9.7727499999999995E-2</v>
-      </c>
-      <c r="J4">
-        <v>9.8786899999999997E-2</v>
-      </c>
-      <c r="K4">
-        <v>9.9106899999999998E-2</v>
-      </c>
-      <c r="L4">
-        <v>9.6954499999999999E-2</v>
-      </c>
-      <c r="M4">
-        <v>9.8385200000000006E-2</v>
-      </c>
-      <c r="N4">
-        <v>9.4825800000000002E-2</v>
-      </c>
-      <c r="O4">
-        <v>9.8732799999999996E-2</v>
-      </c>
-      <c r="P4">
-        <v>9.8261899999999999E-2</v>
-      </c>
-      <c r="Q4">
-        <v>9.9188999999999999E-2</v>
-      </c>
-      <c r="R4">
-        <v>9.9669599999999997E-2</v>
-      </c>
-      <c r="S4">
-        <v>9.9956699999999996E-2</v>
-      </c>
-      <c r="T4">
-        <v>0.10273309999999999</v>
-      </c>
-      <c r="U4">
-        <v>9.7878699999999999E-2</v>
-      </c>
-      <c r="V4">
-        <v>9.9678900000000001E-2</v>
-      </c>
-      <c r="W4">
-        <v>9.9640900000000004E-2</v>
-      </c>
-      <c r="X4">
-        <v>9.9360900000000002E-2</v>
-      </c>
-      <c r="Y4">
-        <v>9.8609699999999995E-2</v>
-      </c>
-      <c r="Z4">
-        <v>9.7461400000000004E-2</v>
-      </c>
-      <c r="AA4">
-        <v>0.1002686</v>
-      </c>
-      <c r="AB4">
-        <v>9.9910299999999994E-2</v>
-      </c>
-      <c r="AC4">
-        <v>9.8755700000000002E-2</v>
-      </c>
-      <c r="AD4">
-        <v>0.1006644</v>
-      </c>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+        <v>0.1084191</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B5">
-        <v>9.3226699999999996E-2</v>
+        <v>0.1031142</v>
       </c>
       <c r="C5">
-        <v>9.7916900000000001E-2</v>
+        <v>9.9625599999999995E-2</v>
       </c>
       <c r="D5">
-        <v>9.6797599999999998E-2</v>
+        <v>0.10336289999999999</v>
       </c>
       <c r="E5">
-        <v>9.7286999999999998E-2</v>
+        <v>0.10262590000000001</v>
       </c>
       <c r="F5">
-        <v>9.8425399999999996E-2</v>
+        <v>9.8684400000000005E-2</v>
       </c>
       <c r="G5">
-        <v>9.6685999999999994E-2</v>
-      </c>
-      <c r="H5">
-        <v>9.9739499999999995E-2</v>
-      </c>
-      <c r="I5">
-        <v>9.7175999999999998E-2</v>
-      </c>
-      <c r="J5">
-        <v>9.8527199999999995E-2</v>
-      </c>
-      <c r="K5">
-        <v>9.8523299999999994E-2</v>
-      </c>
-      <c r="L5">
-        <v>9.9142099999999997E-2</v>
-      </c>
-      <c r="M5">
-        <v>9.5977499999999993E-2</v>
-      </c>
-      <c r="N5">
-        <v>9.8025200000000007E-2</v>
-      </c>
-      <c r="O5">
-        <v>9.7034300000000004E-2</v>
-      </c>
-      <c r="P5">
-        <v>9.6954499999999999E-2</v>
-      </c>
-      <c r="Q5">
-        <v>9.7937300000000005E-2</v>
-      </c>
-      <c r="R5">
-        <v>9.9551799999999996E-2</v>
-      </c>
-      <c r="S5">
-        <v>9.9251599999999995E-2</v>
-      </c>
-      <c r="T5">
-        <v>9.9139199999999997E-2</v>
-      </c>
-      <c r="U5">
-        <v>9.7288700000000006E-2</v>
-      </c>
-      <c r="V5">
-        <v>9.8294199999999998E-2</v>
-      </c>
-      <c r="W5">
-        <v>9.94062E-2</v>
-      </c>
-      <c r="X5">
-        <v>9.9542500000000006E-2</v>
-      </c>
-      <c r="Y5">
-        <v>9.8483100000000004E-2</v>
-      </c>
-      <c r="Z5">
-        <v>9.8900399999999999E-2</v>
-      </c>
-      <c r="AA5">
-        <v>0.10075050000000001</v>
-      </c>
-      <c r="AB5">
-        <v>0.10187110000000001</v>
-      </c>
-      <c r="AC5">
-        <v>9.9099999999999994E-2</v>
-      </c>
-      <c r="AD5">
-        <v>9.9068600000000007E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+        <v>9.9284200000000003E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B6">
-        <v>9.1793200000000005E-2</v>
+        <v>9.8190200000000005E-2</v>
       </c>
       <c r="C6">
-        <v>9.6522899999999995E-2</v>
+        <v>9.8634399999999997E-2</v>
       </c>
       <c r="D6">
-        <v>9.6728099999999997E-2</v>
+        <v>0.1022203</v>
       </c>
       <c r="E6">
-        <v>0.10067130000000001</v>
+        <v>0.1035572</v>
       </c>
       <c r="F6">
-        <v>9.8704600000000003E-2</v>
+        <v>9.9105899999999997E-2</v>
       </c>
       <c r="G6">
-        <v>9.7159400000000007E-2</v>
-      </c>
-      <c r="H6">
-        <v>9.8571500000000006E-2</v>
-      </c>
-      <c r="I6">
-        <v>9.7377199999999997E-2</v>
-      </c>
-      <c r="J6">
-        <v>9.8569000000000004E-2</v>
-      </c>
-      <c r="K6">
-        <v>9.9017999999999995E-2</v>
-      </c>
-      <c r="L6">
-        <v>9.8346900000000001E-2</v>
-      </c>
-      <c r="M6">
-        <v>9.4414399999999996E-2</v>
-      </c>
-      <c r="N6">
-        <v>9.7807199999999997E-2</v>
-      </c>
-      <c r="O6">
-        <v>9.5048800000000003E-2</v>
-      </c>
-      <c r="P6">
-        <v>9.9199599999999999E-2</v>
-      </c>
-      <c r="Q6">
-        <v>9.7856600000000002E-2</v>
-      </c>
-      <c r="R6">
-        <v>9.7611199999999995E-2</v>
-      </c>
-      <c r="S6">
-        <v>9.9477800000000005E-2</v>
-      </c>
-      <c r="T6">
-        <v>9.7639199999999995E-2</v>
-      </c>
-      <c r="U6">
-        <v>9.7213999999999995E-2</v>
-      </c>
-      <c r="V6">
-        <v>9.8115400000000005E-2</v>
-      </c>
-      <c r="W6">
-        <v>9.8062700000000003E-2</v>
-      </c>
-      <c r="X6">
-        <v>9.6425499999999997E-2</v>
-      </c>
-      <c r="Y6">
-        <v>9.84043E-2</v>
-      </c>
-      <c r="Z6">
-        <v>9.7890500000000005E-2</v>
-      </c>
-      <c r="AA6">
-        <v>0.1022033</v>
-      </c>
-      <c r="AB6">
-        <v>9.8653400000000002E-2</v>
-      </c>
-      <c r="AC6">
-        <v>9.7141699999999997E-2</v>
-      </c>
-      <c r="AD6">
-        <v>9.9488699999999999E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+        <v>0.1026537</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B7">
-        <v>9.5120999999999997E-2</v>
+        <v>0.10263360000000001</v>
       </c>
       <c r="C7">
-        <v>9.8949700000000002E-2</v>
+        <v>0.1079644</v>
       </c>
       <c r="D7">
-        <v>9.8329799999999995E-2</v>
+        <v>9.90872E-2</v>
       </c>
       <c r="E7">
-        <v>9.7912100000000002E-2</v>
+        <v>0.10263899999999999</v>
       </c>
       <c r="F7">
-        <v>9.7577800000000006E-2</v>
+        <v>0.1026244</v>
       </c>
       <c r="G7">
-        <v>9.46906E-2</v>
-      </c>
-      <c r="H7">
-        <v>9.6977599999999997E-2</v>
-      </c>
-      <c r="I7">
-        <v>9.6786200000000003E-2</v>
-      </c>
-      <c r="J7">
-        <v>9.9032400000000007E-2</v>
-      </c>
-      <c r="K7">
-        <v>9.7825499999999996E-2</v>
-      </c>
-      <c r="L7">
-        <v>0.1041141</v>
-      </c>
-      <c r="M7">
-        <v>9.9099699999999999E-2</v>
-      </c>
-      <c r="N7">
-        <v>0.1033898</v>
-      </c>
-      <c r="O7">
-        <v>9.7872399999999998E-2</v>
-      </c>
-      <c r="P7">
-        <v>9.8164299999999996E-2</v>
-      </c>
-      <c r="Q7">
-        <v>0.1153081</v>
-      </c>
-      <c r="R7">
-        <v>0.1008879</v>
-      </c>
-      <c r="S7">
-        <v>9.9344299999999996E-2</v>
-      </c>
-      <c r="T7">
-        <v>9.9692500000000003E-2</v>
-      </c>
-      <c r="U7">
-        <v>0.1036984</v>
-      </c>
-      <c r="V7">
-        <v>9.9099000000000007E-2</v>
-      </c>
-      <c r="W7">
-        <v>9.8510600000000004E-2</v>
-      </c>
-      <c r="X7">
-        <v>9.7813999999999998E-2</v>
-      </c>
-      <c r="Y7">
-        <v>9.79965E-2</v>
-      </c>
-      <c r="Z7">
-        <v>0.1001012</v>
-      </c>
-      <c r="AA7">
-        <v>9.8217200000000005E-2</v>
-      </c>
-      <c r="AB7">
-        <v>9.8269400000000007E-2</v>
-      </c>
-      <c r="AC7">
-        <v>0.10072970000000001</v>
-      </c>
-      <c r="AD7">
-        <v>0.1047463</v>
-      </c>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+        <v>0.10220700000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B8">
-        <v>9.7901500000000002E-2</v>
+        <v>0.10304919999999999</v>
       </c>
       <c r="C8">
-        <v>9.59729E-2</v>
+        <v>0.1112677</v>
       </c>
       <c r="D8">
-        <v>0.100713</v>
+        <v>0.10036929999999999</v>
       </c>
       <c r="E8">
-        <v>0.1001967</v>
+        <v>0.1059287</v>
       </c>
       <c r="F8">
-        <v>9.7498000000000001E-2</v>
+        <v>0.11053979999999999</v>
       </c>
       <c r="G8">
-        <v>9.7449099999999997E-2</v>
-      </c>
-      <c r="H8">
-        <v>9.8805000000000004E-2</v>
-      </c>
-      <c r="I8">
-        <v>9.8561999999999997E-2</v>
-      </c>
-      <c r="J8">
-        <v>0.1026233</v>
-      </c>
-      <c r="K8">
-        <v>0.1003114</v>
-      </c>
-      <c r="L8">
-        <v>9.9433300000000002E-2</v>
-      </c>
-      <c r="M8">
-        <v>9.8307900000000004E-2</v>
-      </c>
-      <c r="N8">
-        <v>9.8409899999999995E-2</v>
-      </c>
-      <c r="O8">
-        <v>9.7532999999999995E-2</v>
-      </c>
-      <c r="P8">
-        <v>9.9668099999999996E-2</v>
-      </c>
-      <c r="Q8">
-        <v>0.10010819999999999</v>
-      </c>
-      <c r="R8">
-        <v>0.1058901</v>
-      </c>
-      <c r="S8">
-        <v>0.1005881</v>
-      </c>
-      <c r="T8">
-        <v>0.1003145</v>
-      </c>
-      <c r="U8">
-        <v>0.1003961</v>
-      </c>
-      <c r="V8">
-        <v>0.1016605</v>
-      </c>
-      <c r="W8">
-        <v>9.9451999999999999E-2</v>
-      </c>
-      <c r="X8">
-        <v>9.9829799999999996E-2</v>
-      </c>
-      <c r="Y8">
-        <v>0.1008975</v>
-      </c>
-      <c r="Z8">
-        <v>9.8895399999999994E-2</v>
-      </c>
-      <c r="AA8">
-        <v>0.1010387</v>
-      </c>
-      <c r="AB8">
-        <v>9.9661799999999995E-2</v>
-      </c>
-      <c r="AC8">
-        <v>0.10055939999999999</v>
-      </c>
-      <c r="AD8">
-        <v>0.1014806</v>
-      </c>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+        <v>0.1030445</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B9">
-        <v>0.10171769999999999</v>
+        <v>0.10210950000000001</v>
       </c>
       <c r="C9">
-        <v>9.6668799999999999E-2</v>
+        <v>0.1061696</v>
       </c>
       <c r="D9">
-        <v>9.7072199999999997E-2</v>
+        <v>0.10697669999999999</v>
       </c>
       <c r="E9">
-        <v>0.10276970000000001</v>
+        <v>0.1089933</v>
       </c>
       <c r="F9">
-        <v>9.8947800000000002E-2</v>
+        <v>0.11027389999999999</v>
       </c>
       <c r="G9">
-        <v>0.10078330000000001</v>
-      </c>
-      <c r="H9">
-        <v>0.1003676</v>
-      </c>
-      <c r="I9">
-        <v>0.100428</v>
-      </c>
-      <c r="J9">
-        <v>0.1032068</v>
-      </c>
-      <c r="K9">
-        <v>9.8453299999999994E-2</v>
-      </c>
-      <c r="L9">
-        <v>0.10536909999999999</v>
-      </c>
-      <c r="M9">
-        <v>9.8819900000000002E-2</v>
-      </c>
-      <c r="N9">
-        <v>0.101032</v>
-      </c>
-      <c r="O9">
-        <v>0.10038469999999999</v>
-      </c>
-      <c r="P9">
-        <v>0.1019982</v>
-      </c>
-      <c r="Q9">
-        <v>0.1070501</v>
-      </c>
-      <c r="R9">
-        <v>0.10119209999999999</v>
-      </c>
-      <c r="S9">
-        <v>0.10492360000000001</v>
-      </c>
-      <c r="T9">
-        <v>0.1031966</v>
-      </c>
-      <c r="U9">
-        <v>0.1023014</v>
-      </c>
-      <c r="V9">
-        <v>9.9086499999999994E-2</v>
-      </c>
-      <c r="W9">
-        <v>0.10166500000000001</v>
-      </c>
-      <c r="X9">
-        <v>0.1016976</v>
-      </c>
-      <c r="Y9">
-        <v>0.1025662</v>
-      </c>
-      <c r="Z9">
-        <v>0.1016603</v>
-      </c>
-      <c r="AA9">
-        <v>0.1019055</v>
-      </c>
-      <c r="AB9">
-        <v>0.10408009999999999</v>
-      </c>
-      <c r="AC9">
-        <v>0.1019452</v>
-      </c>
-      <c r="AD9">
-        <v>0.1042872</v>
-      </c>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+        <v>0.120169</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B10">
-        <v>0.1007038</v>
+        <v>0.1051381</v>
       </c>
       <c r="C10">
-        <v>9.35053E-2</v>
+        <v>0.1008395</v>
       </c>
       <c r="D10">
-        <v>0.1005986</v>
+        <v>0.1038917</v>
       </c>
       <c r="E10">
-        <v>9.7327300000000005E-2</v>
+        <v>0.1036487</v>
       </c>
       <c r="F10">
-        <v>9.7912200000000005E-2</v>
+        <v>0.1021654</v>
       </c>
       <c r="G10">
-        <v>9.8516800000000002E-2</v>
-      </c>
-      <c r="H10">
-        <v>9.4547400000000004E-2</v>
-      </c>
-      <c r="I10">
-        <v>9.7014699999999995E-2</v>
-      </c>
-      <c r="J10">
-        <v>0.1038068</v>
-      </c>
-      <c r="K10">
-        <v>0.102257</v>
-      </c>
-      <c r="L10">
-        <v>0.1026514</v>
-      </c>
-      <c r="M10">
-        <v>9.8815500000000001E-2</v>
-      </c>
-      <c r="N10">
-        <v>0.1012349</v>
-      </c>
-      <c r="O10">
-        <v>0.1023265</v>
-      </c>
-      <c r="P10">
-        <v>9.9198700000000001E-2</v>
-      </c>
-      <c r="Q10">
-        <v>0.1091004</v>
-      </c>
-      <c r="R10">
-        <v>9.7965899999999995E-2</v>
-      </c>
-      <c r="S10">
-        <v>0.1034009</v>
-      </c>
-      <c r="T10">
-        <v>0.10341110000000001</v>
-      </c>
-      <c r="U10">
-        <v>0.1022289</v>
-      </c>
-      <c r="V10">
-        <v>9.9697499999999994E-2</v>
-      </c>
-      <c r="W10">
-        <v>0.1024731</v>
-      </c>
-      <c r="X10">
-        <v>9.7073499999999993E-2</v>
-      </c>
-      <c r="Y10">
-        <v>0.1058867</v>
-      </c>
-      <c r="Z10">
-        <v>0.1002484</v>
-      </c>
-      <c r="AA10">
-        <v>0.1028997</v>
-      </c>
-      <c r="AB10">
-        <v>0.103452</v>
-      </c>
-      <c r="AC10">
-        <v>0.1049345</v>
-      </c>
-      <c r="AD10">
-        <v>0.1031571</v>
-      </c>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+        <v>0.1061226</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B11">
-        <v>9.5057699999999995E-2</v>
+        <v>0.11069370000000001</v>
       </c>
       <c r="C11">
-        <v>9.7431100000000007E-2</v>
+        <v>0.1043225</v>
       </c>
       <c r="D11">
-        <v>0.1034137</v>
+        <v>0.1047429</v>
       </c>
       <c r="E11">
-        <v>0.10030849999999999</v>
+        <v>0.1113301</v>
       </c>
       <c r="F11">
-        <v>0.1030288</v>
+        <v>0.104508</v>
       </c>
       <c r="G11">
-        <v>0.1010699</v>
-      </c>
-      <c r="H11">
-        <v>0.1006317</v>
-      </c>
-      <c r="I11">
-        <v>9.8023799999999994E-2</v>
-      </c>
-      <c r="J11">
-        <v>0.1026995</v>
-      </c>
-      <c r="K11">
-        <v>0.1047763</v>
-      </c>
-      <c r="L11">
-        <v>9.9895700000000004E-2</v>
-      </c>
-      <c r="M11">
-        <v>0.10190920000000001</v>
-      </c>
-      <c r="N11">
-        <v>0.10271859999999999</v>
-      </c>
-      <c r="O11">
-        <v>0.10559689999999999</v>
-      </c>
-      <c r="P11">
-        <v>0.10138129999999999</v>
-      </c>
-      <c r="Q11">
-        <v>0.1031849</v>
-      </c>
-      <c r="R11">
-        <v>0.103765</v>
-      </c>
-      <c r="S11">
-        <v>0.1038163</v>
-      </c>
-      <c r="T11">
-        <v>0.102016</v>
-      </c>
-      <c r="U11">
-        <v>0.1025602</v>
-      </c>
-      <c r="V11">
-        <v>0.101773</v>
-      </c>
-      <c r="W11">
-        <v>0.1001745</v>
-      </c>
-      <c r="X11">
-        <v>0.1012072</v>
-      </c>
-      <c r="Y11">
-        <v>0.10245410000000001</v>
-      </c>
-      <c r="Z11">
-        <v>0.1017536</v>
-      </c>
-      <c r="AA11">
-        <v>0.1025731</v>
-      </c>
-      <c r="AB11">
-        <v>0.1046802</v>
-      </c>
-      <c r="AC11">
-        <v>0.1041446</v>
-      </c>
-      <c r="AD11">
-        <v>0.10346229999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+        <v>0.1017358</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B12">
-        <v>9.79101E-2</v>
+        <v>0.102992</v>
       </c>
       <c r="C12">
-        <v>0.10080450000000001</v>
+        <v>0.1036103</v>
       </c>
       <c r="D12">
-        <v>9.5237000000000002E-2</v>
+        <v>0.1042521</v>
       </c>
       <c r="E12">
-        <v>0.1001363</v>
+        <v>0.1048153</v>
       </c>
       <c r="F12">
-        <v>0.1028876</v>
+        <v>0.1068752</v>
       </c>
       <c r="G12">
-        <v>0.101351</v>
-      </c>
-      <c r="H12">
-        <v>0.1031933</v>
-      </c>
-      <c r="I12">
-        <v>0.1023131</v>
-      </c>
-      <c r="J12">
-        <v>0.10205789999999999</v>
-      </c>
-      <c r="K12">
-        <v>0.1027095</v>
-      </c>
-      <c r="L12">
-        <v>0.1006696</v>
-      </c>
-      <c r="M12">
-        <v>0.1014716</v>
-      </c>
-      <c r="N12">
-        <v>0.1030845</v>
-      </c>
-      <c r="O12">
-        <v>0.10462100000000001</v>
-      </c>
-      <c r="P12">
-        <v>0.1019157</v>
-      </c>
-      <c r="Q12">
-        <v>0.10531980000000001</v>
-      </c>
-      <c r="R12">
-        <v>0.1023884</v>
-      </c>
-      <c r="S12">
-        <v>0.1002927</v>
-      </c>
-      <c r="T12">
-        <v>0.1018614</v>
-      </c>
-      <c r="U12">
-        <v>0.10413550000000001</v>
-      </c>
-      <c r="V12">
-        <v>0.10537340000000001</v>
-      </c>
-      <c r="W12">
-        <v>0.10031030000000001</v>
-      </c>
-      <c r="X12">
-        <v>0.1054928</v>
-      </c>
-      <c r="Y12">
-        <v>0.1017855</v>
-      </c>
-      <c r="Z12">
-        <v>0.1007181</v>
-      </c>
-      <c r="AA12">
-        <v>0.1024265</v>
-      </c>
-      <c r="AB12">
-        <v>0.1006296</v>
-      </c>
-      <c r="AC12">
-        <v>0.1047874</v>
-      </c>
-      <c r="AD12">
-        <v>0.1036057</v>
-      </c>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+        <v>0.1216584</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1</v>
       </c>
       <c r="B14">
         <f>SUM(B3:B12)/COUNT(B3:B12)</f>
-        <v>9.6572210000000006E-2</v>
+        <v>0.10337767</v>
       </c>
       <c r="C14">
-        <f t="shared" ref="C14:AD14" si="1">SUM(C3:C12)/COUNT(C3:C12)</f>
-        <v>9.7412849999999995E-2</v>
+        <f>SUM(C3:C12)/COUNT(C3:C12)</f>
+        <v>0.10357288999999999</v>
       </c>
       <c r="D14">
-        <f t="shared" si="1"/>
-        <v>9.8389699999999997E-2</v>
+        <f>SUM(D3:D12)/COUNT(D3:D12)</f>
+        <v>0.10315772000000001</v>
       </c>
       <c r="E14">
-        <f t="shared" si="1"/>
-        <v>9.9235489999999996E-2</v>
+        <f>SUM(E3:E12)/COUNT(E3:E12)</f>
+        <v>0.10491723</v>
       </c>
       <c r="F14">
-        <f t="shared" si="1"/>
-        <v>9.846038E-2</v>
+        <f>SUM(F3:F12)/COUNT(F3:F12)</f>
+        <v>0.10379579999999999</v>
       </c>
       <c r="G14">
-        <f t="shared" si="1"/>
-        <v>9.902161000000001E-2</v>
-      </c>
-      <c r="H14">
-        <f t="shared" si="1"/>
-        <v>9.857883000000002E-2</v>
-      </c>
-      <c r="I14">
-        <f t="shared" si="1"/>
-        <v>9.8140199999999997E-2</v>
-      </c>
-      <c r="J14">
-        <f t="shared" si="1"/>
-        <v>0.10098962</v>
-      </c>
-      <c r="K14">
-        <f t="shared" si="1"/>
-        <v>0.10042429</v>
-      </c>
-      <c r="L14">
-        <f t="shared" si="1"/>
-        <v>0.10095446999999999</v>
-      </c>
-      <c r="M14">
-        <f t="shared" si="1"/>
-        <v>9.8615729999999999E-2</v>
-      </c>
-      <c r="N14">
-        <f t="shared" si="1"/>
-        <v>9.9997720000000012E-2</v>
-      </c>
-      <c r="O14">
-        <f t="shared" si="1"/>
-        <v>9.9785469999999987E-2</v>
-      </c>
-      <c r="P14">
-        <f t="shared" si="1"/>
-        <v>9.9519629999999998E-2</v>
-      </c>
-      <c r="Q14">
-        <f t="shared" si="1"/>
-        <v>0.10331089</v>
-      </c>
-      <c r="R14">
-        <f t="shared" si="1"/>
-        <v>0.10072244999999999</v>
-      </c>
-      <c r="S14">
-        <f t="shared" si="1"/>
-        <v>0.10147857999999998</v>
-      </c>
-      <c r="T14">
-        <f t="shared" si="1"/>
-        <v>0.10131198</v>
-      </c>
-      <c r="U14">
-        <f t="shared" si="1"/>
-        <v>0.10103705999999998</v>
-      </c>
-      <c r="V14">
-        <f t="shared" si="1"/>
-        <v>0.10025352999999999</v>
-      </c>
-      <c r="W14">
-        <f t="shared" si="1"/>
-        <v>0.10012461000000002</v>
-      </c>
-      <c r="X14">
-        <f t="shared" si="1"/>
-        <v>9.9729789999999999E-2</v>
-      </c>
-      <c r="Y14">
-        <f t="shared" si="1"/>
-        <v>0.10068742999999999</v>
-      </c>
-      <c r="Z14">
-        <f t="shared" si="1"/>
-        <v>9.9631440000000002E-2</v>
-      </c>
-      <c r="AA14">
-        <f t="shared" si="1"/>
-        <v>0.10125002000000001</v>
-      </c>
-      <c r="AB14">
-        <f t="shared" si="1"/>
-        <v>0.10132512</v>
-      </c>
-      <c r="AC14">
-        <f t="shared" si="1"/>
-        <v>0.10138329000000001</v>
-      </c>
-      <c r="AD14">
-        <f t="shared" si="1"/>
-        <v>0.10201671999999999</v>
+        <f>SUM(G3:G12)/COUNT(G3:G12)</f>
+        <v>0.10683000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="1">
+        <v>25</v>
+      </c>
+      <c r="C17" s="1">
+        <f>B17+1</f>
+        <v>26</v>
+      </c>
+      <c r="D17" s="1">
+        <f>C17+1</f>
+        <v>27</v>
+      </c>
+      <c r="E17" s="1">
+        <f>D17+1</f>
+        <v>28</v>
+      </c>
+      <c r="F17" s="1">
+        <f>E17+1</f>
+        <v>29</v>
+      </c>
+      <c r="G17" s="1">
+        <f>F17+1</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>0.10337767</v>
+      </c>
+      <c r="C18">
+        <v>0.10357288999999999</v>
+      </c>
+      <c r="D18">
+        <v>0.10315772000000001</v>
+      </c>
+      <c r="E18">
+        <v>0.10491723</v>
+      </c>
+      <c r="F18">
+        <v>0.10379579999999999</v>
+      </c>
+      <c r="G18">
+        <v>0.10683000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A278CDC-E12C-44E3-A607-45211F333E92}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>25</v>
+      </c>
+      <c r="B2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <f>A2+1</f>
+        <v>26</v>
+      </c>
+      <c r="B3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <f>A3+1</f>
+        <v>27</v>
+      </c>
+      <c r="B4">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <f>A4+1</f>
+        <v>28</v>
+      </c>
+      <c r="B5">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <f>A5+1</f>
+        <v>29</v>
+      </c>
+      <c r="B6">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <f>A6+1</f>
+        <v>30</v>
+      </c>
+      <c r="B7">
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added torture test results for BF
</commit_message>
<xml_diff>
--- a/test/Results.xlsx
+++ b/test/Results.xlsx
@@ -3,15 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{250F63CB-4952-43A4-92AF-57BA40C638EF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A63F3A-1AEF-424E-8E5D-5A7B1A26F4E1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2865" yWindow="2850" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DP - Random - Raw results+graph" sheetId="1" r:id="rId1"/>
     <sheet name="DP - Random - Table of results" sheetId="4" r:id="rId2"/>
     <sheet name="BF - Random - Raw results" sheetId="2" r:id="rId3"/>
     <sheet name="BF - Random - Table of results" sheetId="5" r:id="rId4"/>
+    <sheet name="BF - Torture - Raw Data" sheetId="6" r:id="rId5"/>
+    <sheet name="BF - Torture - Table of Results" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="12">
   <si>
     <t xml:space="preserve"> Input n =</t>
   </si>
@@ -62,6 +64,9 @@
   </si>
   <si>
     <t>Average time in milliseconds (BF)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Input nr of edges =</t>
   </si>
 </sst>
 </file>
@@ -105,9 +110,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -3405,8 +3411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD30"/>
   <sheetViews>
-    <sheetView topLeftCell="D7" workbookViewId="0">
-      <selection activeCell="O35" sqref="O35"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection sqref="A1:AD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5352,27 +5358,27 @@
         <v>1</v>
       </c>
       <c r="B14">
-        <f>SUM(B3:B12)/COUNT(B3:B12)</f>
+        <f t="shared" ref="B14:G14" si="0">SUM(B3:B12)/COUNT(B3:B12)</f>
         <v>0.10337767</v>
       </c>
       <c r="C14">
-        <f>SUM(C3:C12)/COUNT(C3:C12)</f>
+        <f t="shared" si="0"/>
         <v>0.10357288999999999</v>
       </c>
       <c r="D14">
-        <f>SUM(D3:D12)/COUNT(D3:D12)</f>
+        <f t="shared" si="0"/>
         <v>0.10315772000000001</v>
       </c>
       <c r="E14">
-        <f>SUM(E3:E12)/COUNT(E3:E12)</f>
+        <f t="shared" si="0"/>
         <v>0.10491723</v>
       </c>
       <c r="F14">
-        <f>SUM(F3:F12)/COUNT(F3:F12)</f>
+        <f t="shared" si="0"/>
         <v>0.10379579999999999</v>
       </c>
       <c r="G14">
-        <f>SUM(G3:G12)/COUNT(G3:G12)</f>
+        <f t="shared" si="0"/>
         <v>0.10683000000000001</v>
       </c>
     </row>
@@ -5437,8 +5443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A278CDC-E12C-44E3-A607-45211F333E92}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5456,7 +5462,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="A2" s="2">
         <v>25</v>
       </c>
       <c r="B2">
@@ -5464,7 +5470,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="A3" s="2">
         <f>A2+1</f>
         <v>26</v>
       </c>
@@ -5473,7 +5479,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="A4" s="2">
         <f>A3+1</f>
         <v>27</v>
       </c>
@@ -5482,7 +5488,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="A5" s="2">
         <f>A4+1</f>
         <v>28</v>
       </c>
@@ -5491,7 +5497,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+      <c r="A6" s="2">
         <f>A5+1</f>
         <v>29</v>
       </c>
@@ -5500,12 +5506,1140 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+      <c r="A7" s="2">
         <f>A6+1</f>
         <v>30</v>
       </c>
       <c r="B7">
         <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3467A519-B1BF-4B46-A6EF-1F421557C5C1}">
+  <dimension ref="A1:AD18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1">
+        <f>B1+1</f>
+        <v>3</v>
+      </c>
+      <c r="D1" s="1">
+        <f t="shared" ref="D1:AD1" si="0">C1+1</f>
+        <v>4</v>
+      </c>
+      <c r="E1" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F1" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="G1" s="1">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H1" s="1">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="I1" s="1">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="J1" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="K1" s="1">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="L1" s="1">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="M1" s="1">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="N1" s="1">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="O1" s="1">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="P1" s="1">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="Q1" s="1">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="R1" s="1">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="S1" s="1">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="T1" s="1">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+      <c r="AD1" s="1"/>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0.10444870000000001</v>
+      </c>
+      <c r="C3">
+        <v>0.1046675</v>
+      </c>
+      <c r="D3">
+        <v>0.1068851</v>
+      </c>
+      <c r="E3">
+        <v>0.10468470000000001</v>
+      </c>
+      <c r="F3">
+        <v>0.1020657</v>
+      </c>
+      <c r="G3">
+        <v>0.1030441</v>
+      </c>
+      <c r="H3">
+        <v>0.1035544</v>
+      </c>
+      <c r="I3">
+        <v>0.1095068</v>
+      </c>
+      <c r="J3">
+        <v>0.10663300000000001</v>
+      </c>
+      <c r="K3">
+        <v>0.1106014</v>
+      </c>
+      <c r="L3">
+        <v>0.1112987</v>
+      </c>
+      <c r="M3">
+        <v>0.14695459999999999</v>
+      </c>
+      <c r="N3">
+        <v>0.2237045</v>
+      </c>
+      <c r="O3">
+        <v>0.41151569999999998</v>
+      </c>
+      <c r="P3">
+        <v>0.72144540000000001</v>
+      </c>
+      <c r="Q3">
+        <v>1.0714128999999999</v>
+      </c>
+      <c r="R3">
+        <v>1.2188648</v>
+      </c>
+      <c r="S3">
+        <v>3.0264419</v>
+      </c>
+      <c r="T3">
+        <v>4.5933695999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0.1011195</v>
+      </c>
+      <c r="C4">
+        <v>0.1032705</v>
+      </c>
+      <c r="D4">
+        <v>0.1029091</v>
+      </c>
+      <c r="E4">
+        <v>0.10567120000000001</v>
+      </c>
+      <c r="F4">
+        <v>0.1033133</v>
+      </c>
+      <c r="G4">
+        <v>0.1022816</v>
+      </c>
+      <c r="H4">
+        <v>0.1013338</v>
+      </c>
+      <c r="I4">
+        <v>0.1124227</v>
+      </c>
+      <c r="J4">
+        <v>0.1035605</v>
+      </c>
+      <c r="K4">
+        <v>0.1065372</v>
+      </c>
+      <c r="L4">
+        <v>0.1179509</v>
+      </c>
+      <c r="M4">
+        <v>0.1258244</v>
+      </c>
+      <c r="N4">
+        <v>0.14822959999999999</v>
+      </c>
+      <c r="O4">
+        <v>0.37496550000000001</v>
+      </c>
+      <c r="P4">
+        <v>0.73242960000000001</v>
+      </c>
+      <c r="Q4">
+        <v>1.1683486000000001</v>
+      </c>
+      <c r="R4">
+        <v>1.1149055999999999</v>
+      </c>
+      <c r="S4">
+        <v>4.1798272000000001</v>
+      </c>
+      <c r="T4">
+        <v>11.436032600000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0.1017282</v>
+      </c>
+      <c r="C5">
+        <v>0.1019935</v>
+      </c>
+      <c r="D5">
+        <v>0.1011469</v>
+      </c>
+      <c r="E5">
+        <v>0.10149270000000001</v>
+      </c>
+      <c r="F5">
+        <v>0.1013651</v>
+      </c>
+      <c r="G5">
+        <v>0.10952779999999999</v>
+      </c>
+      <c r="H5">
+        <v>0.1041146</v>
+      </c>
+      <c r="I5">
+        <v>0.10220170000000001</v>
+      </c>
+      <c r="J5">
+        <v>0.1049052</v>
+      </c>
+      <c r="K5">
+        <v>0.1115628</v>
+      </c>
+      <c r="L5">
+        <v>0.12531690000000001</v>
+      </c>
+      <c r="M5">
+        <v>0.1192894</v>
+      </c>
+      <c r="N5">
+        <v>0.17239489999999999</v>
+      </c>
+      <c r="O5">
+        <v>0.41653129999999999</v>
+      </c>
+      <c r="P5">
+        <v>0.73395180000000004</v>
+      </c>
+      <c r="Q5">
+        <v>0.69094619999999995</v>
+      </c>
+      <c r="R5">
+        <v>2.6353570999999998</v>
+      </c>
+      <c r="S5">
+        <v>4.0036775999999996</v>
+      </c>
+      <c r="T5">
+        <v>9.1187714999999994</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>0.10190829999999999</v>
+      </c>
+      <c r="C6">
+        <v>0.10484250000000001</v>
+      </c>
+      <c r="D6">
+        <v>0.1055174</v>
+      </c>
+      <c r="E6">
+        <v>0.1045065</v>
+      </c>
+      <c r="F6">
+        <v>0.10314420000000001</v>
+      </c>
+      <c r="G6">
+        <v>0.1024076</v>
+      </c>
+      <c r="H6">
+        <v>0.10516730000000001</v>
+      </c>
+      <c r="I6">
+        <v>0.1023917</v>
+      </c>
+      <c r="J6">
+        <v>0.10674980000000001</v>
+      </c>
+      <c r="K6">
+        <v>0.10915329999999999</v>
+      </c>
+      <c r="L6">
+        <v>0.13798730000000001</v>
+      </c>
+      <c r="M6">
+        <v>0.15581680000000001</v>
+      </c>
+      <c r="N6">
+        <v>0.22986989999999999</v>
+      </c>
+      <c r="O6">
+        <v>0.3441649</v>
+      </c>
+      <c r="P6">
+        <v>0.52666210000000002</v>
+      </c>
+      <c r="Q6">
+        <v>1.3971571</v>
+      </c>
+      <c r="R6">
+        <v>1.3617664</v>
+      </c>
+      <c r="S6">
+        <v>4.1929705000000004</v>
+      </c>
+      <c r="T6">
+        <v>7.7314945000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>0.10426820000000001</v>
+      </c>
+      <c r="C7">
+        <v>0.1099107</v>
+      </c>
+      <c r="D7">
+        <v>0.10564220000000001</v>
+      </c>
+      <c r="E7">
+        <v>0.1022497</v>
+      </c>
+      <c r="F7">
+        <v>0.1026444</v>
+      </c>
+      <c r="G7">
+        <v>0.1058757</v>
+      </c>
+      <c r="H7">
+        <v>0.10814699999999999</v>
+      </c>
+      <c r="I7">
+        <v>0.1038563</v>
+      </c>
+      <c r="J7">
+        <v>0.1121432</v>
+      </c>
+      <c r="K7">
+        <v>0.1178879</v>
+      </c>
+      <c r="L7">
+        <v>0.1290114</v>
+      </c>
+      <c r="M7">
+        <v>0.12793009999999999</v>
+      </c>
+      <c r="N7">
+        <v>0.24641379999999999</v>
+      </c>
+      <c r="O7">
+        <v>0.42260259999999999</v>
+      </c>
+      <c r="P7">
+        <v>0.67277750000000003</v>
+      </c>
+      <c r="Q7">
+        <v>0.58254470000000003</v>
+      </c>
+      <c r="R7">
+        <v>2.3256139</v>
+      </c>
+      <c r="S7">
+        <v>4.2236346999999999</v>
+      </c>
+      <c r="T7">
+        <v>4.8879948999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>0.10286339999999999</v>
+      </c>
+      <c r="C8">
+        <v>0.1032452</v>
+      </c>
+      <c r="D8">
+        <v>0.1037969</v>
+      </c>
+      <c r="E8">
+        <v>0.1052916</v>
+      </c>
+      <c r="F8">
+        <v>0.1014893</v>
+      </c>
+      <c r="G8">
+        <v>0.10258399999999999</v>
+      </c>
+      <c r="H8">
+        <v>0.1053249</v>
+      </c>
+      <c r="I8">
+        <v>0.1063253</v>
+      </c>
+      <c r="J8">
+        <v>0.11311069999999999</v>
+      </c>
+      <c r="K8">
+        <v>0.11810519999999999</v>
+      </c>
+      <c r="L8">
+        <v>0.1214964</v>
+      </c>
+      <c r="M8">
+        <v>0.16536380000000001</v>
+      </c>
+      <c r="N8">
+        <v>0.1871826</v>
+      </c>
+      <c r="O8">
+        <v>0.33584069999999999</v>
+      </c>
+      <c r="P8">
+        <v>0.61702199999999996</v>
+      </c>
+      <c r="Q8">
+        <v>1.0594482999999999</v>
+      </c>
+      <c r="R8">
+        <v>2.2241873000000001</v>
+      </c>
+      <c r="S8">
+        <v>3.7190482</v>
+      </c>
+      <c r="T8">
+        <v>4.3705105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>0.1043076</v>
+      </c>
+      <c r="C9">
+        <v>0.10554810000000001</v>
+      </c>
+      <c r="D9">
+        <v>0.10210379999999999</v>
+      </c>
+      <c r="E9">
+        <v>0.1040088</v>
+      </c>
+      <c r="F9">
+        <v>0.10234260000000001</v>
+      </c>
+      <c r="G9">
+        <v>0.10671509999999999</v>
+      </c>
+      <c r="H9">
+        <v>0.1052635</v>
+      </c>
+      <c r="I9">
+        <v>0.110411</v>
+      </c>
+      <c r="J9">
+        <v>0.1110413</v>
+      </c>
+      <c r="K9">
+        <v>0.11579449999999999</v>
+      </c>
+      <c r="L9">
+        <v>0.1223404</v>
+      </c>
+      <c r="M9">
+        <v>0.14060690000000001</v>
+      </c>
+      <c r="N9">
+        <v>0.1488622</v>
+      </c>
+      <c r="O9">
+        <v>0.2726653</v>
+      </c>
+      <c r="P9">
+        <v>0.58281369999999999</v>
+      </c>
+      <c r="Q9">
+        <v>0.59901959999999999</v>
+      </c>
+      <c r="R9">
+        <v>2.3612321000000001</v>
+      </c>
+      <c r="S9">
+        <v>3.6952242000000002</v>
+      </c>
+      <c r="T9">
+        <v>8.2672381999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>0.1045016</v>
+      </c>
+      <c r="C10">
+        <v>0.10378560000000001</v>
+      </c>
+      <c r="D10">
+        <v>0.10534540000000001</v>
+      </c>
+      <c r="E10">
+        <v>0.10784779999999999</v>
+      </c>
+      <c r="F10">
+        <v>0.1033987</v>
+      </c>
+      <c r="G10">
+        <v>0.1035515</v>
+      </c>
+      <c r="H10">
+        <v>0.10624649999999999</v>
+      </c>
+      <c r="I10">
+        <v>0.103883</v>
+      </c>
+      <c r="J10">
+        <v>0.1116553</v>
+      </c>
+      <c r="K10">
+        <v>0.1141221</v>
+      </c>
+      <c r="L10">
+        <v>0.12680040000000001</v>
+      </c>
+      <c r="M10">
+        <v>0.14111370000000001</v>
+      </c>
+      <c r="N10">
+        <v>0.25539869999999998</v>
+      </c>
+      <c r="O10">
+        <v>0.26841140000000002</v>
+      </c>
+      <c r="P10">
+        <v>0.68151079999999997</v>
+      </c>
+      <c r="Q10">
+        <v>1.1571045</v>
+      </c>
+      <c r="R10">
+        <v>1.8140050000000001</v>
+      </c>
+      <c r="S10">
+        <v>3.9937201999999998</v>
+      </c>
+      <c r="T10">
+        <v>9.5886265000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>0.1065354</v>
+      </c>
+      <c r="C11">
+        <v>0.104161</v>
+      </c>
+      <c r="D11">
+        <v>0.1032467</v>
+      </c>
+      <c r="E11">
+        <v>0.1055687</v>
+      </c>
+      <c r="F11">
+        <v>0.1105665</v>
+      </c>
+      <c r="G11">
+        <v>0.1052712</v>
+      </c>
+      <c r="H11">
+        <v>0.1026844</v>
+      </c>
+      <c r="I11">
+        <v>0.104323</v>
+      </c>
+      <c r="J11">
+        <v>0.1093437</v>
+      </c>
+      <c r="K11">
+        <v>0.1187243</v>
+      </c>
+      <c r="L11">
+        <v>0.1227052</v>
+      </c>
+      <c r="M11">
+        <v>0.16916320000000001</v>
+      </c>
+      <c r="N11">
+        <v>0.144651</v>
+      </c>
+      <c r="O11">
+        <v>0.41249950000000002</v>
+      </c>
+      <c r="P11">
+        <v>0.54303789999999996</v>
+      </c>
+      <c r="Q11">
+        <v>1.2121922000000001</v>
+      </c>
+      <c r="R11">
+        <v>1.9299952</v>
+      </c>
+      <c r="S11">
+        <v>1.9075637000000001</v>
+      </c>
+      <c r="T11">
+        <v>3.5325565999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>0.10676380000000001</v>
+      </c>
+      <c r="C12">
+        <v>0.1136818</v>
+      </c>
+      <c r="D12">
+        <v>0.10577549999999999</v>
+      </c>
+      <c r="E12">
+        <v>0.1093441</v>
+      </c>
+      <c r="F12">
+        <v>0.1090434</v>
+      </c>
+      <c r="G12">
+        <v>0.106183</v>
+      </c>
+      <c r="H12">
+        <v>0.1101453</v>
+      </c>
+      <c r="I12">
+        <v>0.1056913</v>
+      </c>
+      <c r="J12">
+        <v>0.10578319999999999</v>
+      </c>
+      <c r="K12">
+        <v>0.1164282</v>
+      </c>
+      <c r="L12">
+        <v>0.13939770000000001</v>
+      </c>
+      <c r="M12">
+        <v>0.1636572</v>
+      </c>
+      <c r="N12">
+        <v>0.2288644</v>
+      </c>
+      <c r="O12">
+        <v>0.23397999999999999</v>
+      </c>
+      <c r="P12">
+        <v>0.42934689999999998</v>
+      </c>
+      <c r="Q12">
+        <v>0.95821719999999999</v>
+      </c>
+      <c r="R12">
+        <v>1.1899332</v>
+      </c>
+      <c r="S12">
+        <v>2.8187163000000002</v>
+      </c>
+      <c r="T12">
+        <v>7.7275016000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <f>SUM(B3:B12)/COUNT(B3:B12)</f>
+        <v>0.10384446999999999</v>
+      </c>
+      <c r="C14">
+        <f t="shared" ref="C14:AD14" si="1">SUM(C3:C12)/COUNT(C3:C12)</f>
+        <v>0.10551064000000002</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>0.10423689999999999</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>0.10506658000000002</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>0.10393731999999997</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>0.10474416</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>0.10519817000000001</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="1"/>
+        <v>0.10610127999999999</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="1"/>
+        <v>0.10849259000000003</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="1"/>
+        <v>0.11389169000000003</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="1"/>
+        <v>0.12543053000000001</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="1"/>
+        <v>0.14557201000000003</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="1"/>
+        <v>0.19855715999999998</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="1"/>
+        <v>0.34931769000000001</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="1"/>
+        <v>0.62409976999999994</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="1"/>
+        <v>0.98963912999999992</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="1"/>
+        <v>1.81758606</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="1"/>
+        <v>3.5760824499999999</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="1"/>
+        <v>7.1254096499999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2</v>
+      </c>
+      <c r="C17" s="1">
+        <f>B17+1</f>
+        <v>3</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" ref="D17" si="2">C17+1</f>
+        <v>4</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" ref="E17" si="3">D17+1</f>
+        <v>5</v>
+      </c>
+      <c r="F17" s="1">
+        <f t="shared" ref="F17" si="4">E17+1</f>
+        <v>6</v>
+      </c>
+      <c r="G17" s="1">
+        <f t="shared" ref="G17" si="5">F17+1</f>
+        <v>7</v>
+      </c>
+      <c r="H17" s="1">
+        <f t="shared" ref="H17" si="6">G17+1</f>
+        <v>8</v>
+      </c>
+      <c r="I17" s="1">
+        <f t="shared" ref="I17" si="7">H17+1</f>
+        <v>9</v>
+      </c>
+      <c r="J17" s="1">
+        <f t="shared" ref="J17" si="8">I17+1</f>
+        <v>10</v>
+      </c>
+      <c r="K17" s="1">
+        <f t="shared" ref="K17" si="9">J17+1</f>
+        <v>11</v>
+      </c>
+      <c r="L17" s="1">
+        <f t="shared" ref="L17" si="10">K17+1</f>
+        <v>12</v>
+      </c>
+      <c r="M17" s="1">
+        <f t="shared" ref="M17" si="11">L17+1</f>
+        <v>13</v>
+      </c>
+      <c r="N17" s="1">
+        <f t="shared" ref="N17" si="12">M17+1</f>
+        <v>14</v>
+      </c>
+      <c r="O17" s="1">
+        <f t="shared" ref="O17" si="13">N17+1</f>
+        <v>15</v>
+      </c>
+      <c r="P17" s="1">
+        <f t="shared" ref="P17" si="14">O17+1</f>
+        <v>16</v>
+      </c>
+      <c r="Q17" s="1">
+        <f t="shared" ref="Q17" si="15">P17+1</f>
+        <v>17</v>
+      </c>
+      <c r="R17" s="1">
+        <f t="shared" ref="R17" si="16">Q17+1</f>
+        <v>18</v>
+      </c>
+      <c r="S17" s="1">
+        <f t="shared" ref="S17" si="17">R17+1</f>
+        <v>19</v>
+      </c>
+      <c r="T17" s="1">
+        <f t="shared" ref="T17" si="18">S17+1</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <f>SUM(B7:B16)/COUNT(B7:B16)</f>
+        <v>0.10472635285714285</v>
+      </c>
+      <c r="C18">
+        <f t="shared" ref="C18:T18" si="19">SUM(C7:C16)/COUNT(C7:C16)</f>
+        <v>0.1065490057142857</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="19"/>
+        <v>0.10430677142857143</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="19"/>
+        <v>0.10562532571428571</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="19"/>
+        <v>0.10477460285714287</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="19"/>
+        <v>0.10498923714285714</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="19"/>
+        <v>0.10614425285714287</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="19"/>
+        <v>0.10579874</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="19"/>
+        <v>0.11022428428571429</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="19"/>
+        <v>0.11642198428571428</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="19"/>
+        <v>0.12674029000000001</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="19"/>
+        <v>0.15048670142857143</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="19"/>
+        <v>0.20141855142857143</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="19"/>
+        <v>0.32790245571428572</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="19"/>
+        <v>0.59294408142857136</v>
+      </c>
+      <c r="Q18">
+        <f t="shared" si="19"/>
+        <v>0.93688080428571419</v>
+      </c>
+      <c r="R18">
+        <f t="shared" si="19"/>
+        <v>1.9517932514285714</v>
+      </c>
+      <c r="S18">
+        <f t="shared" si="19"/>
+        <v>3.419141392857143</v>
+      </c>
+      <c r="T18">
+        <f t="shared" si="19"/>
+        <v>6.4999768500000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B752322-E4FC-4074-964D-8B0F19C80E33}">
+  <dimension ref="A1:C20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="35" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>1952</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>3419</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>6500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Results updated with 2 larger instances of BF torture
</commit_message>
<xml_diff>
--- a/test/Results.xlsx
+++ b/test/Results.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A63F3A-1AEF-424E-8E5D-5A7B1A26F4E1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A84003-90E8-4E1B-84E7-54E8BEBFB04E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4841,8 +4841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86B2FD24-48B6-4D33-AC11-A86A9E1FB876}">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection sqref="A1:B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5103,7 +5103,7 @@
   <dimension ref="A1:X18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:G18"/>
+      <selection activeCell="I17" sqref="I17:I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5136,7 +5136,9 @@
         <v>30</v>
       </c>
       <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
+      <c r="I1" s="1">
+        <v>2</v>
+      </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
@@ -5172,6 +5174,9 @@
       <c r="G3">
         <v>0.10300570000000001</v>
       </c>
+      <c r="I3">
+        <v>0.18670809999999999</v>
+      </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B4">
@@ -5192,6 +5197,9 @@
       <c r="G4">
         <v>0.1084191</v>
       </c>
+      <c r="I4">
+        <v>0.10439329999999999</v>
+      </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B5">
@@ -5212,6 +5220,9 @@
       <c r="G5">
         <v>9.9284200000000003E-2</v>
       </c>
+      <c r="I5">
+        <v>0.1069809</v>
+      </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B6">
@@ -5232,6 +5243,9 @@
       <c r="G6">
         <v>0.1026537</v>
       </c>
+      <c r="I6">
+        <v>0.1162498</v>
+      </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B7">
@@ -5252,6 +5266,9 @@
       <c r="G7">
         <v>0.10220700000000001</v>
       </c>
+      <c r="I7">
+        <v>9.8600699999999999E-2</v>
+      </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B8">
@@ -5272,6 +5289,9 @@
       <c r="G8">
         <v>0.1030445</v>
       </c>
+      <c r="I8">
+        <v>0.11506139999999999</v>
+      </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B9">
@@ -5292,6 +5312,9 @@
       <c r="G9">
         <v>0.120169</v>
       </c>
+      <c r="I9">
+        <v>9.9273200000000006E-2</v>
+      </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B10">
@@ -5312,6 +5335,9 @@
       <c r="G10">
         <v>0.1061226</v>
       </c>
+      <c r="I10">
+        <v>9.8701399999999995E-2</v>
+      </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B11">
@@ -5332,6 +5358,9 @@
       <c r="G11">
         <v>0.1017358</v>
       </c>
+      <c r="I11">
+        <v>0.1058784</v>
+      </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B12">
@@ -5352,13 +5381,16 @@
       <c r="G12">
         <v>0.1216584</v>
       </c>
+      <c r="I12">
+        <v>0.1058895</v>
+      </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1</v>
       </c>
       <c r="B14">
-        <f t="shared" ref="B14:G14" si="0">SUM(B3:B12)/COUNT(B3:B12)</f>
+        <f t="shared" ref="B14:I14" si="0">SUM(B3:B12)/COUNT(B3:B12)</f>
         <v>0.10337767</v>
       </c>
       <c r="C14">
@@ -5381,8 +5413,12 @@
         <f t="shared" si="0"/>
         <v>0.10683000000000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>0.11377366999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
@@ -5409,8 +5445,11 @@
         <f>F17+1</f>
         <v>30</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I17" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -5431,6 +5470,9 @@
       </c>
       <c r="G18">
         <v>0.10683000000000001</v>
+      </c>
+      <c r="I18">
+        <v>0.11377366999999998</v>
       </c>
     </row>
   </sheetData>
@@ -5441,10 +5483,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A278CDC-E12C-44E3-A607-45211F333E92}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A7"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5514,6 +5556,15 @@
         <v>107</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <f>114</f>
+        <v>114</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5525,7 +5576,7 @@
   <dimension ref="A1:AD18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+      <selection activeCell="U17" sqref="U17:V18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5542,7 +5593,7 @@
         <v>3</v>
       </c>
       <c r="D1" s="1">
-        <f t="shared" ref="D1:AD1" si="0">C1+1</f>
+        <f t="shared" ref="D1:T1" si="0">C1+1</f>
         <v>4</v>
       </c>
       <c r="E1" s="1">
@@ -5609,8 +5660,14 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
+      <c r="U1" s="1">
+        <f t="shared" ref="U1" si="1">T1+1</f>
+        <v>21</v>
+      </c>
+      <c r="V1" s="1">
+        <f t="shared" ref="V1" si="2">U1+1</f>
+        <v>22</v>
+      </c>
       <c r="W1" s="1"/>
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
@@ -5681,6 +5738,12 @@
       <c r="T3">
         <v>4.5933695999999999</v>
       </c>
+      <c r="U3">
+        <v>17.4981002</v>
+      </c>
+      <c r="V3">
+        <v>27.533467900000002</v>
+      </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -5743,6 +5806,12 @@
       <c r="T4">
         <v>11.436032600000001</v>
       </c>
+      <c r="U4">
+        <v>18.083905399999999</v>
+      </c>
+      <c r="V4">
+        <v>15.7433022</v>
+      </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -5805,6 +5874,12 @@
       <c r="T5">
         <v>9.1187714999999994</v>
       </c>
+      <c r="U5">
+        <v>19.010254199999999</v>
+      </c>
+      <c r="V5">
+        <v>42.615857300000002</v>
+      </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B6">
@@ -5864,6 +5939,12 @@
       <c r="T6">
         <v>7.7314945000000002</v>
       </c>
+      <c r="U6">
+        <v>20.526265899999999</v>
+      </c>
+      <c r="V6">
+        <v>43.449876000000003</v>
+      </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B7">
@@ -5923,6 +6004,12 @@
       <c r="T7">
         <v>4.8879948999999998</v>
       </c>
+      <c r="U7">
+        <v>18.921216300000001</v>
+      </c>
+      <c r="V7">
+        <v>37.087336999999998</v>
+      </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B8">
@@ -5982,6 +6069,12 @@
       <c r="T8">
         <v>4.3705105</v>
       </c>
+      <c r="U8">
+        <v>16.451014900000001</v>
+      </c>
+      <c r="V8">
+        <v>19.721128</v>
+      </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B9">
@@ -6041,6 +6134,12 @@
       <c r="T9">
         <v>8.2672381999999995</v>
       </c>
+      <c r="U9">
+        <v>15.7355491</v>
+      </c>
+      <c r="V9">
+        <v>36.030599500000001</v>
+      </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B10">
@@ -6100,6 +6199,12 @@
       <c r="T10">
         <v>9.5886265000000002</v>
       </c>
+      <c r="U10">
+        <v>16.244662699999999</v>
+      </c>
+      <c r="V10">
+        <v>20.189039699999999</v>
+      </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B11">
@@ -6159,6 +6264,12 @@
       <c r="T11">
         <v>3.5325565999999999</v>
       </c>
+      <c r="U11">
+        <v>19.714613700000001</v>
+      </c>
+      <c r="V11">
+        <v>39.988544599999997</v>
+      </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B12">
@@ -6218,6 +6329,12 @@
       <c r="T12">
         <v>7.7275016000000001</v>
       </c>
+      <c r="U12">
+        <v>13.299252299999999</v>
+      </c>
+      <c r="V12">
+        <v>46.027616100000003</v>
+      </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -6228,79 +6345,87 @@
         <v>0.10384446999999999</v>
       </c>
       <c r="C14">
-        <f t="shared" ref="C14:AD14" si="1">SUM(C3:C12)/COUNT(C3:C12)</f>
+        <f t="shared" ref="C14:W14" si="3">SUM(C3:C12)/COUNT(C3:C12)</f>
         <v>0.10551064000000002</v>
       </c>
       <c r="D14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.10423689999999999</v>
       </c>
       <c r="E14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.10506658000000002</v>
       </c>
       <c r="F14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.10393731999999997</v>
       </c>
       <c r="G14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.10474416</v>
       </c>
       <c r="H14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.10519817000000001</v>
       </c>
       <c r="I14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.10610127999999999</v>
       </c>
       <c r="J14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.10849259000000003</v>
       </c>
       <c r="K14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.11389169000000003</v>
       </c>
       <c r="L14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.12543053000000001</v>
       </c>
       <c r="M14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.14557201000000003</v>
       </c>
       <c r="N14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.19855715999999998</v>
       </c>
       <c r="O14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.34931769000000001</v>
       </c>
       <c r="P14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.62409976999999994</v>
       </c>
       <c r="Q14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.98963912999999992</v>
       </c>
       <c r="R14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.81758606</v>
       </c>
       <c r="S14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.5760824499999999</v>
       </c>
       <c r="T14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.1254096499999999</v>
       </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U14">
+        <f t="shared" si="3"/>
+        <v>17.548483470000001</v>
+      </c>
+      <c r="V14">
+        <f t="shared" si="3"/>
+        <v>32.838676829999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
@@ -6312,75 +6437,81 @@
         <v>3</v>
       </c>
       <c r="D17" s="1">
-        <f t="shared" ref="D17" si="2">C17+1</f>
+        <f t="shared" ref="D17" si="4">C17+1</f>
         <v>4</v>
       </c>
       <c r="E17" s="1">
-        <f t="shared" ref="E17" si="3">D17+1</f>
+        <f t="shared" ref="E17" si="5">D17+1</f>
         <v>5</v>
       </c>
       <c r="F17" s="1">
-        <f t="shared" ref="F17" si="4">E17+1</f>
+        <f t="shared" ref="F17" si="6">E17+1</f>
         <v>6</v>
       </c>
       <c r="G17" s="1">
-        <f t="shared" ref="G17" si="5">F17+1</f>
+        <f t="shared" ref="G17" si="7">F17+1</f>
         <v>7</v>
       </c>
       <c r="H17" s="1">
-        <f t="shared" ref="H17" si="6">G17+1</f>
+        <f t="shared" ref="H17" si="8">G17+1</f>
         <v>8</v>
       </c>
       <c r="I17" s="1">
-        <f t="shared" ref="I17" si="7">H17+1</f>
+        <f t="shared" ref="I17" si="9">H17+1</f>
         <v>9</v>
       </c>
       <c r="J17" s="1">
-        <f t="shared" ref="J17" si="8">I17+1</f>
+        <f t="shared" ref="J17" si="10">I17+1</f>
         <v>10</v>
       </c>
       <c r="K17" s="1">
-        <f t="shared" ref="K17" si="9">J17+1</f>
+        <f t="shared" ref="K17" si="11">J17+1</f>
         <v>11</v>
       </c>
       <c r="L17" s="1">
-        <f t="shared" ref="L17" si="10">K17+1</f>
+        <f t="shared" ref="L17" si="12">K17+1</f>
         <v>12</v>
       </c>
       <c r="M17" s="1">
-        <f t="shared" ref="M17" si="11">L17+1</f>
+        <f t="shared" ref="M17" si="13">L17+1</f>
         <v>13</v>
       </c>
       <c r="N17" s="1">
-        <f t="shared" ref="N17" si="12">M17+1</f>
+        <f t="shared" ref="N17" si="14">M17+1</f>
         <v>14</v>
       </c>
       <c r="O17" s="1">
-        <f t="shared" ref="O17" si="13">N17+1</f>
+        <f t="shared" ref="O17" si="15">N17+1</f>
         <v>15</v>
       </c>
       <c r="P17" s="1">
-        <f t="shared" ref="P17" si="14">O17+1</f>
+        <f t="shared" ref="P17" si="16">O17+1</f>
         <v>16</v>
       </c>
       <c r="Q17" s="1">
-        <f t="shared" ref="Q17" si="15">P17+1</f>
+        <f t="shared" ref="Q17" si="17">P17+1</f>
         <v>17</v>
       </c>
       <c r="R17" s="1">
-        <f t="shared" ref="R17" si="16">Q17+1</f>
+        <f t="shared" ref="R17" si="18">Q17+1</f>
         <v>18</v>
       </c>
       <c r="S17" s="1">
-        <f t="shared" ref="S17" si="17">R17+1</f>
+        <f t="shared" ref="S17" si="19">R17+1</f>
         <v>19</v>
       </c>
       <c r="T17" s="1">
-        <f t="shared" ref="T17" si="18">S17+1</f>
+        <f t="shared" ref="T17" si="20">S17+1</f>
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U17" s="1">
+        <v>21</v>
+      </c>
+      <c r="V17" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -6389,89 +6520,96 @@
         <v>0.10472635285714285</v>
       </c>
       <c r="C18">
-        <f t="shared" ref="C18:T18" si="19">SUM(C7:C16)/COUNT(C7:C16)</f>
+        <f t="shared" ref="C18:T18" si="21">SUM(C7:C16)/COUNT(C7:C16)</f>
         <v>0.1065490057142857</v>
       </c>
       <c r="D18">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>0.10430677142857143</v>
       </c>
       <c r="E18">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>0.10562532571428571</v>
       </c>
       <c r="F18">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>0.10477460285714287</v>
       </c>
       <c r="G18">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>0.10498923714285714</v>
       </c>
       <c r="H18">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>0.10614425285714287</v>
       </c>
       <c r="I18">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>0.10579874</v>
       </c>
       <c r="J18">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>0.11022428428571429</v>
       </c>
       <c r="K18">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>0.11642198428571428</v>
       </c>
       <c r="L18">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>0.12674029000000001</v>
       </c>
       <c r="M18">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>0.15048670142857143</v>
       </c>
       <c r="N18">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>0.20141855142857143</v>
       </c>
       <c r="O18">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>0.32790245571428572</v>
       </c>
       <c r="P18">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>0.59294408142857136</v>
       </c>
       <c r="Q18">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>0.93688080428571419</v>
       </c>
       <c r="R18">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>1.9517932514285714</v>
       </c>
       <c r="S18">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>3.419141392857143</v>
       </c>
       <c r="T18">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>6.4999768500000004</v>
+      </c>
+      <c r="U18">
+        <v>17.548483470000001</v>
+      </c>
+      <c r="V18">
+        <v>32.838676829999997</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B752322-E4FC-4074-964D-8B0F19C80E33}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A21" sqref="A21:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6642,6 +6780,22 @@
         <v>6500</v>
       </c>
     </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>17548</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>22</v>
+      </c>
+      <c r="B22">
+        <v>32839</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>